<commit_message>
Update VZ Consolidated IS,BS, & CF .xlsx
Fixed Excel project error
</commit_message>
<xml_diff>
--- a/Projects/VZ Consolidated IS,BS, & CF .xlsx
+++ b/Projects/VZ Consolidated IS,BS, & CF .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\FineLit\FineLit Portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\de59.github.io\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D38125-8767-415B-9B2F-E5C11C94B415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3359F079-DA50-4CBF-95C0-E70E3B57322F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A25086B5-4036-4D1C-9EF2-0F45196E0FB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A25086B5-4036-4D1C-9EF2-0F45196E0FB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="9" r:id="rId1"/>
@@ -45,7 +45,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId9"/>
     <pivotCache cacheId="1" r:id="rId10"/>
-    <pivotCache cacheId="8" r:id="rId11"/>
+    <pivotCache cacheId="2" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2343,10 +2343,30 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="13" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="43" fontId="13" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2362,14 +2382,20 @@
     <xf numFmtId="9" fontId="26" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2382,18 +2408,21 @@
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="4" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2403,40 +2432,11 @@
     <xf numFmtId="44" fontId="4" fillId="4" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="6" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="13" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2447,65 +2447,7 @@
   </cellStyles>
   <dxfs count="63">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri Light"/>
-        <family val="1"/>
-        <scheme val="major"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF5B960"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -2723,13 +2665,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color auto="1"/>
         </right>
@@ -2742,7 +2677,72 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri Light"/>
+        <family val="1"/>
+        <scheme val="major"/>
+      </font>
+      <numFmt numFmtId="167" formatCode="yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFF5B960"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -13169,7 +13169,130 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BBD0F0-4AF2-43DD-9BCF-BED90A89C91C}" name="PivotTable1" cacheId="8" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98A09A1D-A604-4DDC-A3C5-5C0FA55D5081}" name="PivotTable9" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Trend Analysis Balance Sheet" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A12:C17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="26">
+        <item h="1" x="10"/>
+        <item h="1" x="2"/>
+        <item h="1" x="21"/>
+        <item x="0"/>
+        <item h="1" x="18"/>
+        <item h="1" x="6"/>
+        <item h="1" x="7"/>
+        <item h="1" x="1"/>
+        <item h="1" x="13"/>
+        <item h="1" x="22"/>
+        <item h="1" x="8"/>
+        <item h="1" x="11"/>
+        <item h="1" x="14"/>
+        <item h="1" x="17"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="19"/>
+        <item h="1" x="9"/>
+        <item h="1" x="4"/>
+        <item h="1" x="12"/>
+        <item h="1" x="23"/>
+        <item h="1" x="16"/>
+        <item h="1" x="24"/>
+        <item h="1" x="15"/>
+        <item h="1" x="20"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="4">
+    <dataField name="2016A" fld="1" baseField="2" baseItem="0"/>
+    <dataField name="2017A" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="2018A" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="2019A" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="3">
+    <chartFormat chart="3" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42BBD0F0-4AF2-43DD-9BCF-BED90A89C91C}" name="PivotTable1" cacheId="2" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="H10:M15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -13492,7 +13615,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FA439A93-8D5E-4CBB-BBB1-A39CE4B742BB}" name="PivotTable6" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Commonsized Balance Sheet" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A3:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -13574,7 +13697,7 @@
     <dataField name="2016A" fld="1" subtotal="max" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="10">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -13647,129 +13770,6 @@
           </reference>
           <reference field="0" count="1" selected="0">
             <x v="19"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{98A09A1D-A604-4DDC-A3C5-5C0FA55D5081}" name="PivotTable9" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Trend Analysis Balance Sheet" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A12:C17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisCol" showAll="0">
-      <items count="26">
-        <item h="1" x="10"/>
-        <item h="1" x="2"/>
-        <item h="1" x="21"/>
-        <item x="0"/>
-        <item h="1" x="18"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="1"/>
-        <item h="1" x="13"/>
-        <item h="1" x="22"/>
-        <item h="1" x="8"/>
-        <item h="1" x="11"/>
-        <item h="1" x="14"/>
-        <item h="1" x="17"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="19"/>
-        <item h="1" x="9"/>
-        <item h="1" x="4"/>
-        <item h="1" x="12"/>
-        <item h="1" x="23"/>
-        <item h="1" x="16"/>
-        <item h="1" x="24"/>
-        <item h="1" x="15"/>
-        <item h="1" x="20"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="0"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="4">
-    <dataField name="2016A" fld="1" baseField="2" baseItem="0"/>
-    <dataField name="2017A" fld="2" baseField="0" baseItem="0"/>
-    <dataField name="2018A" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="2019A" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="3">
-    <chartFormat chart="3" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
           </reference>
         </references>
       </pivotArea>
@@ -13929,14 +13929,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D851BEB4-F57E-48BA-BB2A-07865D762AE7}" name="Ratios" displayName="Ratios" ref="B92:F116" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D851BEB4-F57E-48BA-BB2A-07865D762AE7}" name="Ratios" displayName="Ratios" ref="B92:F116" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B92:F116" xr:uid="{4AC246CB-1B8B-4074-B7A8-72CB43500BB3}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A868839B-2AD6-4F91-A8AB-34953C47ED7E}" name="Ratios" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{0EB71E22-E538-4C39-96E7-AB082023E69F}" name="2016" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{7724D99C-FE3C-4A19-8D46-AC3227CE314C}" name="2017" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{9D38E68A-1C29-4B65-A586-2F042473F665}" name="2018" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{9788D129-700F-46BE-B46C-55AF3A23585F}" name="2019" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A868839B-2AD6-4F91-A8AB-34953C47ED7E}" name="Ratios" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0EB71E22-E538-4C39-96E7-AB082023E69F}" name="2016" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{7724D99C-FE3C-4A19-8D46-AC3227CE314C}" name="2017" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9D38E68A-1C29-4B65-A586-2F042473F665}" name="2018" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9788D129-700F-46BE-B46C-55AF3A23585F}" name="2019" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14241,7 +14241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5A38D5E-E30A-49FE-AF3D-C4B640654F45}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -14253,112 +14253,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
-      <c r="A1" s="305" t="s">
+      <c r="A1" s="304" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="305"/>
-      <c r="C1" s="305"/>
-      <c r="D1" s="305"/>
-      <c r="E1" s="305"/>
-      <c r="F1" s="305"/>
+      <c r="B1" s="304"/>
+      <c r="C1" s="304"/>
+      <c r="D1" s="304"/>
+      <c r="E1" s="304"/>
+      <c r="F1" s="304"/>
       <c r="G1" s="263"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1">
-      <c r="A2" s="305"/>
-      <c r="B2" s="305"/>
-      <c r="C2" s="305"/>
-      <c r="D2" s="305"/>
-      <c r="E2" s="305"/>
-      <c r="F2" s="305"/>
+      <c r="A2" s="304"/>
+      <c r="B2" s="304"/>
+      <c r="C2" s="304"/>
+      <c r="D2" s="304"/>
+      <c r="E2" s="304"/>
+      <c r="F2" s="304"/>
       <c r="G2" s="263"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1">
-      <c r="A3" s="306" t="s">
+      <c r="A3" s="305" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="306"/>
-      <c r="C3" s="306"/>
-      <c r="D3" s="298" t="s">
+      <c r="B3" s="305"/>
+      <c r="C3" s="305"/>
+      <c r="D3" s="307" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="298"/>
+      <c r="E3" s="307"/>
       <c r="F3" s="263"/>
       <c r="G3" s="263"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="306" t="s">
+      <c r="A4" s="305" t="s">
         <v>222</v>
       </c>
-      <c r="B4" s="306"/>
-      <c r="C4" s="306"/>
-      <c r="D4" s="298" t="s">
+      <c r="B4" s="305"/>
+      <c r="C4" s="305"/>
+      <c r="D4" s="307" t="s">
         <v>228</v>
       </c>
-      <c r="E4" s="298"/>
+      <c r="E4" s="307"/>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A5" s="299" t="s">
+      <c r="A5" s="306" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="299"/>
-      <c r="C5" s="299"/>
-      <c r="D5" s="301">
+      <c r="B5" s="306"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="309">
         <v>61.5</v>
       </c>
-      <c r="E5" s="301"/>
+      <c r="E5" s="309"/>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A6" s="299" t="s">
+      <c r="A6" s="306" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="299"/>
-      <c r="C6" s="299"/>
-      <c r="D6" s="302">
+      <c r="B6" s="306"/>
+      <c r="C6" s="306"/>
+      <c r="D6" s="310">
         <f>DCF!H1</f>
-        <v>-43.570493844620025</v>
-      </c>
-      <c r="E6" s="303"/>
+        <v>68.04644895076774</v>
+      </c>
+      <c r="E6" s="311"/>
     </row>
     <row r="7" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A7" s="299" t="s">
+      <c r="A7" s="306" t="s">
         <v>225</v>
       </c>
-      <c r="B7" s="299"/>
-      <c r="C7" s="299"/>
-      <c r="D7" s="304">
+      <c r="B7" s="306"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="312">
         <f>DCF!H2</f>
-        <v>-1.708463314546667</v>
-      </c>
-      <c r="E7" s="298"/>
+        <v>0.10644632440272749</v>
+      </c>
+      <c r="E7" s="307"/>
     </row>
     <row r="8" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A8" s="299" t="s">
+      <c r="A8" s="306" t="s">
         <v>226</v>
       </c>
-      <c r="B8" s="299"/>
-      <c r="C8" s="299"/>
-      <c r="D8" s="298">
+      <c r="B8" s="306"/>
+      <c r="C8" s="306"/>
+      <c r="D8" s="307">
         <v>3</v>
       </c>
-      <c r="E8" s="298"/>
+      <c r="E8" s="307"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="300" t="str">
+      <c r="A9" s="308" t="str">
         <f>DCF!B5</f>
         <v>(1-Above Avg., 2-Slightly Above Avg., 3-Base, 4-Slightly Below Avg., 5-Below Average)</v>
       </c>
-      <c r="B9" s="300"/>
-      <c r="C9" s="300"/>
+      <c r="B9" s="308"/>
+      <c r="C9" s="308"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="300"/>
-      <c r="B10" s="300"/>
-      <c r="C10" s="300"/>
+      <c r="A10" s="308"/>
+      <c r="B10" s="308"/>
+      <c r="C10" s="308"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="300"/>
-      <c r="B11" s="300"/>
-      <c r="C11" s="300"/>
+      <c r="A11" s="308"/>
+      <c r="B11" s="308"/>
+      <c r="C11" s="308"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="138" t="s">
@@ -14404,11 +14404,6 @@
     </scenario>
   </scenarios>
   <mergeCells count="14">
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
@@ -14418,6 +14413,11 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14428,8 +14428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6446CE3F-FD5D-41FF-80D9-682EF99159B7}">
   <dimension ref="A1:S92"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14449,23 +14449,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="309" t="s">
+      <c r="A1" s="323" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="309"/>
+      <c r="B1" s="323"/>
       <c r="C1" s="152">
         <f>Dashboard!D5</f>
         <v>61.5</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="312" t="s">
+      <c r="F1" s="326" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="312"/>
+      <c r="G1" s="326"/>
       <c r="H1" s="116">
         <f>Target_Price</f>
-        <v>-43.570493844620025</v>
+        <v>68.04644895076774</v>
       </c>
       <c r="I1" s="15"/>
       <c r="J1" s="124"/>
@@ -14480,23 +14480,23 @@
       <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="309" t="s">
+      <c r="A2" s="323" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="309"/>
+      <c r="B2" s="323"/>
       <c r="C2" s="154">
         <f>'Consolidated Financials'!P18</f>
         <v>4140</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
-      <c r="F2" s="312" t="s">
+      <c r="F2" s="326" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="312"/>
+      <c r="G2" s="326"/>
       <c r="H2" s="117">
         <f>(H1-C1)/C1</f>
-        <v>-1.708463314546667</v>
+        <v>0.10644632440272749</v>
       </c>
       <c r="I2" s="15"/>
       <c r="J2" s="124"/>
@@ -14511,10 +14511,10 @@
       <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="309" t="s">
+      <c r="A3" s="323" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="309"/>
+      <c r="B3" s="323"/>
       <c r="C3" s="120">
         <f>N29</f>
         <v>8.2784699519411836E-2</v>
@@ -14537,10 +14537,10 @@
       <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="309" t="s">
+      <c r="A4" s="323" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="309"/>
+      <c r="B4" s="323"/>
       <c r="C4" s="121">
         <f>N20</f>
         <v>9.8672464583656166E-2</v>
@@ -14622,10 +14622,10 @@
         <v>161</v>
       </c>
       <c r="K6" s="13"/>
-      <c r="L6" s="310" t="s">
+      <c r="L6" s="324" t="s">
         <v>153</v>
       </c>
-      <c r="M6" s="311"/>
+      <c r="M6" s="325"/>
       <c r="N6" s="15" t="s">
         <v>154</v>
       </c>
@@ -14647,54 +14647,54 @@
       </c>
       <c r="B7" s="222"/>
       <c r="C7" s="223"/>
-      <c r="D7" s="224" t="e">
-        <f>RevenueY1</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E7" s="224" t="e">
-        <f>RevenueY2</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F7" s="224" t="e">
-        <f>RevenueY3</f>
-        <v>#NAME?</v>
+      <c r="D7" s="224">
+        <f>'Consolidated Financials'!I6</f>
+        <v>126034</v>
+      </c>
+      <c r="E7" s="224">
+        <f>'Consolidated Financials'!J6</f>
+        <v>130863</v>
+      </c>
+      <c r="F7" s="224">
+        <f>'Consolidated Financials'!K6</f>
+        <v>131868</v>
       </c>
       <c r="G7" s="225">
         <f>IFERROR(F7*(1+G8), 0)</f>
-        <v>0</v>
+        <v>134900.62411682113</v>
       </c>
       <c r="H7" s="225">
         <f>IFERROR(G7*(1+H8), 0)</f>
-        <v>0</v>
+        <v>136969.81149147992</v>
       </c>
       <c r="I7" s="225">
         <f>IFERROR(H7*(1+I8), 0)</f>
-        <v>0</v>
+        <v>139595.25071834619</v>
       </c>
       <c r="J7" s="226">
         <f>IFERROR(I7*(1+J8), 0)</f>
-        <v>0</v>
+        <v>142003.73075798561</v>
       </c>
       <c r="K7" s="13"/>
-      <c r="L7" s="310" t="s">
+      <c r="L7" s="324" t="s">
         <v>107</v>
       </c>
-      <c r="M7" s="311"/>
+      <c r="M7" s="325"/>
       <c r="N7" s="122">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="O7" s="146" t="e">
+      <c r="O7" s="146">
         <f>D7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="P7" s="146" t="e">
+        <v>126034</v>
+      </c>
+      <c r="P7" s="146">
         <f>E7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="Q7" s="146" t="e">
+        <v>130863</v>
+      </c>
+      <c r="Q7" s="146">
         <f>F7</f>
-        <v>#NAME?</v>
+        <v>131868</v>
       </c>
       <c r="R7" s="15"/>
       <c r="S7" s="13"/>
@@ -14708,33 +14708,33 @@
       <c r="D8" s="230"/>
       <c r="E8" s="230">
         <f>IFERROR((E7-D7)/D7,0)</f>
-        <v>0</v>
+        <v>3.8315057841534821E-2</v>
       </c>
       <c r="F8" s="230">
         <f>IFERROR((F7-E7)/E7,0)</f>
-        <v>0</v>
+        <v>7.6797872584305725E-3</v>
       </c>
       <c r="G8" s="231">
         <f>+CHOOSE($G$4,(IFERROR(SUM(E8:F8)/2, 0))*1.25,(IFERROR(SUM(E8:F8)/2, 0))*1.1,(IFERROR(SUM(E8:F8)/2, 0)),(IFERROR(SUM(E8:F8)/2, 0))*0.9, (IFERROR(SUM(E8:F8)/2, 0))*0.75)</f>
-        <v>0</v>
+        <v>2.2997422549982695E-2</v>
       </c>
       <c r="H8" s="231">
         <f>+CHOOSE($G$4,(IFERROR(SUM(F8:G8)/2, 0))*1.25,(IFERROR(SUM(F8:G8)/2, 0))*1.1,(IFERROR(SUM(F8:G8)/2, 0)),(IFERROR(SUM(F8:G8)/2, 0))*0.9, (IFERROR(SUM(F8:G8)/2, 0))*0.75)</f>
-        <v>0</v>
+        <v>1.5338604904206634E-2</v>
       </c>
       <c r="I8" s="231">
         <f>+CHOOSE($G$4,(IFERROR(SUM(G8:H8)/2, 0))*1.25,(IFERROR(SUM(G8:H8)/2, 0))*1.1,(IFERROR(SUM(G8:H8)/2, 0)),(IFERROR(SUM(G8:H8)/2, 0))*0.9, (IFERROR(SUM(G8:H8)/2, 0))*0.75)</f>
-        <v>0</v>
+        <v>1.9168013727094663E-2</v>
       </c>
       <c r="J8" s="232">
         <f>+CHOOSE($G$4,(IFERROR(SUM(H8:I8)/2, 0))*1.25,(IFERROR(SUM(H8:I8)/2, 0))*1.1,(IFERROR(SUM(H8:I8)/2, 0)),(IFERROR(SUM(H8:I8)/2, 0))*0.9, (IFERROR(SUM(H8:I8)/2, 0))*0.75)</f>
-        <v>0</v>
+        <v>1.7253309315650649E-2</v>
       </c>
       <c r="K8" s="13"/>
-      <c r="L8" s="307" t="s">
+      <c r="L8" s="320" t="s">
         <v>17</v>
       </c>
-      <c r="M8" s="308"/>
+      <c r="M8" s="321"/>
       <c r="N8" s="122"/>
       <c r="O8" s="122">
         <f>'Consolidated Financials'!I17</f>
@@ -14771,25 +14771,25 @@
       </c>
       <c r="G9" s="235">
         <f>IFERROR(G$7*G10, 0)</f>
-        <v>0</v>
+        <v>34597.504156022449</v>
       </c>
       <c r="H9" s="235">
         <f>IFERROR(H7*H10, 0)</f>
-        <v>0</v>
+        <v>34950.136726302742</v>
       </c>
       <c r="I9" s="235">
         <f>IFERROR(I7*I10, 0)</f>
-        <v>0</v>
+        <v>36046.355062481685</v>
       </c>
       <c r="J9" s="236">
         <f>IFERROR(J7*J10, 0)</f>
-        <v>0</v>
+        <v>36440.704364385259</v>
       </c>
       <c r="K9" s="13"/>
-      <c r="L9" s="307" t="s">
+      <c r="L9" s="320" t="s">
         <v>164</v>
       </c>
-      <c r="M9" s="308"/>
+      <c r="M9" s="321"/>
       <c r="N9" s="122"/>
       <c r="O9" s="122">
         <f>'Consolidated Financials'!I14*(-1)</f>
@@ -14812,39 +14812,39 @@
         <v>165</v>
       </c>
       <c r="C10" s="230"/>
-      <c r="D10" s="230" t="e">
+      <c r="D10" s="230">
         <f>D9/D7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E10" s="230" t="e">
+        <v>0.26036625037688244</v>
+      </c>
+      <c r="E10" s="230">
         <f>E9/E7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F10" s="230" t="e">
+        <v>0.24600536438871187</v>
+      </c>
+      <c r="F10" s="230">
         <f>F9/F7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G10" s="238" t="e">
+        <v>0.26302817969484638</v>
+      </c>
+      <c r="G10" s="238">
         <f>SUM(D10:F10)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H10" s="238" t="e">
+        <v>0.25646659815348022</v>
+      </c>
+      <c r="H10" s="238">
         <f>SUM(E10:G10)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I10" s="238" t="e">
+        <v>0.25516671407901281</v>
+      </c>
+      <c r="I10" s="238">
         <f>SUM(F10:H10)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J10" s="239" t="e">
+        <v>0.25822049730911312</v>
+      </c>
+      <c r="J10" s="239">
         <f>SUM(G10:I10)/3</f>
-        <v>#NAME?</v>
+        <v>0.25661793651386872</v>
       </c>
       <c r="K10" s="13"/>
-      <c r="L10" s="307" t="s">
+      <c r="L10" s="320" t="s">
         <v>166</v>
       </c>
-      <c r="M10" s="308"/>
+      <c r="M10" s="321"/>
       <c r="N10" s="122"/>
       <c r="O10" s="122">
         <f>'Consolidated Financials'!I12</f>
@@ -14881,25 +14881,25 @@
       </c>
       <c r="G11" s="235">
         <f>IFERROR(G$7*G12, 0)</f>
-        <v>0</v>
+        <v>16880.06288693257</v>
       </c>
       <c r="H11" s="235">
         <f>IFERROR(H$7*H12, 0)</f>
-        <v>0</v>
+        <v>17106.226336575575</v>
       </c>
       <c r="I11" s="235">
         <f>IFERROR(I$7*I12, 0)</f>
-        <v>0</v>
+        <v>17986.521662483545</v>
       </c>
       <c r="J11" s="236">
         <f>IFERROR(J$7*J12, 0)</f>
-        <v>0</v>
+        <v>17933.545172285703</v>
       </c>
       <c r="K11" s="13"/>
-      <c r="L11" s="307" t="s">
+      <c r="L11" s="320" t="s">
         <v>168</v>
       </c>
-      <c r="M11" s="308"/>
+      <c r="M11" s="321"/>
       <c r="N11" s="122"/>
       <c r="O11" s="122">
         <f>'Consolidated Financials'!I9</f>
@@ -14922,33 +14922,33 @@
         <v>165</v>
       </c>
       <c r="C12" s="230"/>
-      <c r="D12" s="230" t="e">
+      <c r="D12" s="230">
         <f>D11/D7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E12" s="230" t="e">
+        <v>0.12584699366837521</v>
+      </c>
+      <c r="E12" s="230">
         <f>E11/E7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F12" s="230" t="e">
+        <v>0.11301895875839618</v>
+      </c>
+      <c r="F12" s="230">
         <f>F11/F7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G12" s="238" t="e">
+        <v>0.13652288652288652</v>
+      </c>
+      <c r="G12" s="238">
         <f>SUM(D12:F12)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H12" s="238" t="e">
+        <v>0.12512961298321931</v>
+      </c>
+      <c r="H12" s="238">
         <f>SUM(E12:G12)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I12" s="238" t="e">
+        <v>0.12489048608816733</v>
+      </c>
+      <c r="I12" s="238">
         <f>SUM(F12:H12)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J12" s="239" t="e">
+        <v>0.12884766186475771</v>
+      </c>
+      <c r="J12" s="239">
         <f>SUM(G12:I12)/3</f>
-        <v>#NAME?</v>
+        <v>0.12628925364538146</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="125"/>
@@ -14992,25 +14992,25 @@
       </c>
       <c r="G13" s="235">
         <f>IFERROR(G$7*G14, 0)</f>
-        <v>0</v>
+        <v>17717.441269089879</v>
       </c>
       <c r="H13" s="235">
         <f>IFERROR(H$7*H14, 0)</f>
-        <v>0</v>
+        <v>17843.910389727167</v>
       </c>
       <c r="I13" s="235">
         <f>IFERROR(I$7*I14, 0)</f>
-        <v>0</v>
+        <v>18059.833399998137</v>
       </c>
       <c r="J13" s="236">
         <f>IFERROR(J$7*J14, 0)</f>
-        <v>0</v>
+        <v>18507.15919209956</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="L13" s="307" t="s">
+      <c r="L13" s="320" t="s">
         <v>170</v>
       </c>
-      <c r="M13" s="308"/>
+      <c r="M13" s="321"/>
       <c r="N13" s="123">
         <f>'Consolidated Financials'!C10</f>
         <v>84751</v>
@@ -15036,39 +15036,39 @@
         <v>171</v>
       </c>
       <c r="C14" s="230"/>
-      <c r="D14" s="230" t="e">
+      <c r="D14" s="230">
         <f>D13/D7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E14" s="230" t="e">
+        <v>0.13451925670850723</v>
+      </c>
+      <c r="E14" s="230">
         <f>E13/E7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F14" s="230" t="e">
+        <v>0.13298640563031566</v>
+      </c>
+      <c r="F14" s="230">
         <f>F13/F7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G14" s="238" t="e">
+        <v>0.12650529317195983</v>
+      </c>
+      <c r="G14" s="238">
         <f>SUM(D14:F14)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H14" s="238" t="e">
+        <v>0.13133698517026091</v>
+      </c>
+      <c r="H14" s="238">
         <f>SUM(E14:G14)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I14" s="238" t="e">
+        <v>0.13027622799084548</v>
+      </c>
+      <c r="I14" s="238">
         <f>SUM(F14:H14)/3</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J14" s="239" t="e">
+        <v>0.12937283544435541</v>
+      </c>
+      <c r="J14" s="239">
         <f>SUM(G14:I14)/3</f>
-        <v>#NAME?</v>
+        <v>0.13032868286848728</v>
       </c>
       <c r="K14" s="13"/>
-      <c r="L14" s="307" t="s">
+      <c r="L14" s="320" t="s">
         <v>185</v>
       </c>
-      <c r="M14" s="308"/>
+      <c r="M14" s="321"/>
       <c r="N14" s="123"/>
       <c r="O14" s="148">
         <f>ABS(O10/D37)</f>
@@ -15385,7 +15385,7 @@
       <c r="M21" s="126"/>
       <c r="N21" s="131">
         <f>J59*(1-N19)</f>
-        <v>-11445.487338294157</v>
+        <v>22898.862456405994</v>
       </c>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
@@ -15434,7 +15434,7 @@
       <c r="M22" s="126"/>
       <c r="N22" s="131">
         <f>N21/(N20-N19)</f>
-        <v>-141002.09223656703</v>
+        <v>282101.35757066333</v>
       </c>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
@@ -15486,7 +15486,7 @@
       <c r="M23" s="126"/>
       <c r="N23" s="131">
         <f>N22/((1+N20)^J44)</f>
-        <v>-88081.429852433968</v>
+        <v>176223.5619628118</v>
       </c>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
@@ -16265,7 +16265,7 @@
       <c r="M42" s="126"/>
       <c r="N42" s="131">
         <f>N23+F17+C62+F19+F27</f>
-        <v>-79669.844516726909</v>
+        <v>382424.29865617846</v>
       </c>
       <c r="O42" s="15"/>
       <c r="P42" s="15"/>
@@ -16310,10 +16310,10 @@
       <c r="S43" s="13"/>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="314" t="s">
+      <c r="A44" s="322" t="s">
         <v>202</v>
       </c>
-      <c r="B44" s="314"/>
+      <c r="B44" s="322"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
@@ -16339,7 +16339,7 @@
       <c r="M44" s="126"/>
       <c r="N44" s="131">
         <f>N42-N43</f>
-        <v>-180381.84451672691</v>
+        <v>281712.29865617846</v>
       </c>
       <c r="O44" s="15"/>
       <c r="P44" s="15"/>
@@ -16348,32 +16348,32 @@
       <c r="S44" s="13"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="313" t="s">
+      <c r="A45" s="318" t="s">
         <v>204</v>
       </c>
-      <c r="B45" s="313"/>
+      <c r="B45" s="318"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
-      <c r="F45" s="139" t="e">
+      <c r="F45" s="139">
         <f>F7</f>
-        <v>#NAME?</v>
+        <v>131868</v>
       </c>
       <c r="G45" s="139">
         <f>G7</f>
-        <v>0</v>
+        <v>134900.62411682113</v>
       </c>
       <c r="H45" s="139">
         <f>H7</f>
-        <v>0</v>
+        <v>136969.81149147992</v>
       </c>
       <c r="I45" s="139">
         <f>I7</f>
-        <v>0</v>
+        <v>139595.25071834619</v>
       </c>
       <c r="J45" s="140">
         <f>J7</f>
-        <v>0</v>
+        <v>142003.73075798561</v>
       </c>
       <c r="K45" s="13"/>
       <c r="L45" s="125" t="s">
@@ -16391,10 +16391,10 @@
       <c r="S45" s="13"/>
     </row>
     <row r="46" spans="1:19">
-      <c r="A46" s="313" t="s">
+      <c r="A46" s="318" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="313"/>
+      <c r="B46" s="318"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
@@ -16404,19 +16404,19 @@
       </c>
       <c r="G46" s="139">
         <f>G9</f>
-        <v>0</v>
+        <v>34597.504156022449</v>
       </c>
       <c r="H46" s="139">
         <f>H9</f>
-        <v>0</v>
+        <v>34950.136726302742</v>
       </c>
       <c r="I46" s="139">
         <f>I9</f>
-        <v>0</v>
+        <v>36046.355062481685</v>
       </c>
       <c r="J46" s="140">
         <f>J9</f>
-        <v>0</v>
+        <v>36440.704364385259</v>
       </c>
       <c r="K46" s="13"/>
       <c r="L46" s="127" t="s">
@@ -16425,7 +16425,7 @@
       <c r="M46" s="128"/>
       <c r="N46" s="133">
         <f>IFERROR(N44/N45,0)</f>
-        <v>-43.570493844620025</v>
+        <v>68.04644895076774</v>
       </c>
       <c r="O46" s="15"/>
       <c r="P46" s="15"/>
@@ -16434,10 +16434,10 @@
       <c r="S46" s="13"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="313" t="s">
+      <c r="A47" s="318" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="313"/>
+      <c r="B47" s="318"/>
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -16447,19 +16447,19 @@
       </c>
       <c r="G47" s="139">
         <f>G11</f>
-        <v>0</v>
+        <v>16880.06288693257</v>
       </c>
       <c r="H47" s="139">
         <f>H11</f>
-        <v>0</v>
+        <v>17106.226336575575</v>
       </c>
       <c r="I47" s="139">
         <f>I11</f>
-        <v>0</v>
+        <v>17986.521662483545</v>
       </c>
       <c r="J47" s="140">
         <f>J11</f>
-        <v>0</v>
+        <v>17933.545172285703</v>
       </c>
       <c r="K47" s="13"/>
       <c r="L47" s="125"/>
@@ -16472,10 +16472,10 @@
       <c r="S47" s="13"/>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" s="313" t="s">
+      <c r="A48" s="318" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="313"/>
+      <c r="B48" s="318"/>
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
@@ -16510,10 +16510,10 @@
       <c r="S48" s="13"/>
     </row>
     <row r="49" spans="1:19">
-      <c r="A49" s="313" t="s">
+      <c r="A49" s="318" t="s">
         <v>206</v>
       </c>
-      <c r="B49" s="313"/>
+      <c r="B49" s="318"/>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
@@ -16523,19 +16523,19 @@
       </c>
       <c r="G49" s="109">
         <f t="shared" ref="G49:J49" si="41">G47*(1-G48)</f>
-        <v>0</v>
+        <v>15482.651952969083</v>
       </c>
       <c r="H49" s="109">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>15690.092529391117</v>
       </c>
       <c r="I49" s="109">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>16497.512871255454</v>
       </c>
       <c r="J49" s="142">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>16448.922023880234</v>
       </c>
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
@@ -16548,10 +16548,10 @@
       <c r="S49" s="13"/>
     </row>
     <row r="50" spans="1:19">
-      <c r="A50" s="313" t="s">
+      <c r="A50" s="318" t="s">
         <v>169</v>
       </c>
-      <c r="B50" s="313"/>
+      <c r="B50" s="318"/>
       <c r="C50" s="15"/>
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
@@ -16561,19 +16561,19 @@
       </c>
       <c r="G50" s="139">
         <f>G13</f>
-        <v>0</v>
+        <v>17717.441269089879</v>
       </c>
       <c r="H50" s="139">
         <f>H13</f>
-        <v>0</v>
+        <v>17843.910389727167</v>
       </c>
       <c r="I50" s="139">
         <f>I13</f>
-        <v>0</v>
+        <v>18059.833399998137</v>
       </c>
       <c r="J50" s="140">
         <f>J13</f>
-        <v>0</v>
+        <v>18507.15919209956</v>
       </c>
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
@@ -16586,10 +16586,10 @@
       <c r="S50" s="13"/>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" s="313" t="s">
+      <c r="A51" s="318" t="s">
         <v>207</v>
       </c>
-      <c r="B51" s="313"/>
+      <c r="B51" s="318"/>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
@@ -16624,10 +16624,10 @@
       <c r="S51" s="13"/>
     </row>
     <row r="52" spans="1:19">
-      <c r="A52" s="313" t="s">
+      <c r="A52" s="318" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="313"/>
+      <c r="B52" s="318"/>
       <c r="C52" s="15"/>
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
@@ -16662,10 +16662,10 @@
       <c r="S52" s="13"/>
     </row>
     <row r="53" spans="1:19">
-      <c r="A53" s="313" t="s">
+      <c r="A53" s="318" t="s">
         <v>180</v>
       </c>
-      <c r="B53" s="313"/>
+      <c r="B53" s="318"/>
       <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
@@ -16700,10 +16700,10 @@
       <c r="S53" s="13"/>
     </row>
     <row r="54" spans="1:19">
-      <c r="A54" s="313" t="s">
+      <c r="A54" s="318" t="s">
         <v>208</v>
       </c>
-      <c r="B54" s="313"/>
+      <c r="B54" s="318"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
@@ -16738,10 +16738,10 @@
       <c r="S54" s="13"/>
     </row>
     <row r="55" spans="1:19">
-      <c r="A55" s="313" t="s">
+      <c r="A55" s="318" t="s">
         <v>126</v>
       </c>
-      <c r="B55" s="313"/>
+      <c r="B55" s="318"/>
       <c r="C55" s="15"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
@@ -16776,10 +16776,10 @@
       <c r="S55" s="13"/>
     </row>
     <row r="56" spans="1:19">
-      <c r="A56" s="313" t="s">
+      <c r="A56" s="318" t="s">
         <v>188</v>
       </c>
-      <c r="B56" s="313"/>
+      <c r="B56" s="318"/>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
@@ -16814,10 +16814,10 @@
       <c r="S56" s="13"/>
     </row>
     <row r="57" spans="1:19">
-      <c r="A57" s="313" t="s">
+      <c r="A57" s="318" t="s">
         <v>209</v>
       </c>
-      <c r="B57" s="313"/>
+      <c r="B57" s="318"/>
       <c r="C57" s="15"/>
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
@@ -16852,10 +16852,10 @@
       <c r="S57" s="13"/>
     </row>
     <row r="58" spans="1:19">
-      <c r="A58" s="313" t="s">
+      <c r="A58" s="318" t="s">
         <v>210</v>
       </c>
-      <c r="B58" s="313"/>
+      <c r="B58" s="318"/>
       <c r="C58" s="15"/>
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
@@ -16890,10 +16890,10 @@
       <c r="S58" s="13"/>
     </row>
     <row r="59" spans="1:19">
-      <c r="A59" s="315" t="s">
+      <c r="A59" s="319" t="s">
         <v>211</v>
       </c>
-      <c r="B59" s="315"/>
+      <c r="B59" s="319"/>
       <c r="C59" s="119"/>
       <c r="D59" s="119"/>
       <c r="E59" s="119"/>
@@ -16903,19 +16903,19 @@
       </c>
       <c r="G59" s="143">
         <f>SUM(G49:G58)</f>
-        <v>-4412.3134320398576</v>
+        <v>28787.779790019104</v>
       </c>
       <c r="H59" s="143">
         <f t="shared" ref="H59:I59" si="50">SUM(H49:H58)</f>
-        <v>-6462.5348106316433</v>
+        <v>27071.46810848665</v>
       </c>
       <c r="I59" s="143">
         <f t="shared" si="50"/>
-        <v>-10097.868726494637</v>
+        <v>24459.477544758956</v>
       </c>
       <c r="J59" s="144">
         <f>SUM(J49:J58)</f>
-        <v>-11649.350980452067</v>
+        <v>23306.730235527728</v>
       </c>
       <c r="K59" s="13"/>
       <c r="L59" s="13"/>
@@ -16928,10 +16928,10 @@
       <c r="S59" s="13"/>
     </row>
     <row r="60" spans="1:19">
-      <c r="A60" s="313" t="s">
+      <c r="A60" s="318" t="s">
         <v>212</v>
       </c>
-      <c r="B60" s="313"/>
+      <c r="B60" s="318"/>
       <c r="C60" s="15"/>
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
@@ -16966,10 +16966,10 @@
       <c r="S60" s="13"/>
     </row>
     <row r="61" spans="1:19">
-      <c r="A61" s="313" t="s">
+      <c r="A61" s="318" t="s">
         <v>213</v>
       </c>
-      <c r="B61" s="313"/>
+      <c r="B61" s="318"/>
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
@@ -16979,19 +16979,19 @@
       </c>
       <c r="G61" s="139">
         <f t="shared" ref="G61:J61" si="52">G59/(1-G60)^G44</f>
-        <v>-5431.2660540375555</v>
+        <v>35435.853221414291</v>
       </c>
       <c r="H61" s="139">
         <f t="shared" si="52"/>
-        <v>-8825.8182291277462</v>
+        <v>36971.229358496763</v>
       </c>
       <c r="I61" s="139">
         <f t="shared" si="52"/>
-        <v>-15300.272471496692</v>
+        <v>37060.956235581711</v>
       </c>
       <c r="J61" s="140">
         <f t="shared" si="52"/>
-        <v>-19583.419888190332</v>
+        <v>39180.335899314494</v>
       </c>
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
@@ -17004,13 +17004,13 @@
       <c r="S61" s="13"/>
     </row>
     <row r="62" spans="1:19">
-      <c r="A62" s="317" t="s">
+      <c r="A62" s="316" t="s">
         <v>214</v>
       </c>
-      <c r="B62" s="317"/>
+      <c r="B62" s="316"/>
       <c r="C62" s="268">
         <f>SUM(F61:J61)</f>
-        <v>-19611.414664292937</v>
+        <v>178177.73669336666</v>
       </c>
       <c r="D62" s="130"/>
       <c r="E62" s="130"/>
@@ -17029,8 +17029,8 @@
       <c r="S62" s="13"/>
     </row>
     <row r="63" spans="1:19">
-      <c r="A63" s="318"/>
-      <c r="B63" s="318"/>
+      <c r="A63" s="317"/>
+      <c r="B63" s="317"/>
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
       <c r="E63" s="13"/>
@@ -17050,140 +17050,179 @@
       <c r="S63" s="13"/>
     </row>
     <row r="64" spans="1:19">
-      <c r="A64" s="319"/>
-      <c r="B64" s="319"/>
+      <c r="A64" s="313"/>
+      <c r="B64" s="313"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="319"/>
-      <c r="B65" s="319"/>
+      <c r="A65" s="313"/>
+      <c r="B65" s="313"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="316"/>
-      <c r="B66" s="316"/>
+      <c r="A66" s="314"/>
+      <c r="B66" s="314"/>
       <c r="C66" s="110"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="316"/>
-      <c r="B67" s="316"/>
+      <c r="A67" s="314"/>
+      <c r="B67" s="314"/>
       <c r="C67" s="111"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="316"/>
-      <c r="B68" s="316"/>
+      <c r="A68" s="314"/>
+      <c r="B68" s="314"/>
       <c r="C68" s="112"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="316"/>
-      <c r="B69" s="316"/>
+      <c r="A69" s="314"/>
+      <c r="B69" s="314"/>
       <c r="C69" s="112"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="316"/>
-      <c r="B70" s="316"/>
+      <c r="A70" s="314"/>
+      <c r="B70" s="314"/>
       <c r="C70" s="112"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="319"/>
-      <c r="B72" s="319"/>
+      <c r="A72" s="313"/>
+      <c r="B72" s="313"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="316"/>
-      <c r="B73" s="316"/>
+      <c r="A73" s="314"/>
+      <c r="B73" s="314"/>
       <c r="C73" s="112"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="316"/>
-      <c r="B74" s="316"/>
+      <c r="A74" s="314"/>
+      <c r="B74" s="314"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="316"/>
-      <c r="B75" s="316"/>
+      <c r="A75" s="314"/>
+      <c r="B75" s="314"/>
       <c r="C75" s="111"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="316"/>
-      <c r="B76" s="316"/>
+      <c r="A76" s="314"/>
+      <c r="B76" s="314"/>
       <c r="C76" s="113"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="316"/>
-      <c r="B77" s="316"/>
+      <c r="A77" s="314"/>
+      <c r="B77" s="314"/>
       <c r="C77" s="111"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="316"/>
-      <c r="B78" s="316"/>
+      <c r="A78" s="314"/>
+      <c r="B78" s="314"/>
       <c r="C78" s="111"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="316"/>
-      <c r="B80" s="316"/>
+      <c r="A80" s="314"/>
+      <c r="B80" s="314"/>
       <c r="C80" s="114"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="316"/>
-      <c r="B81" s="316"/>
+      <c r="A81" s="314"/>
+      <c r="B81" s="314"/>
       <c r="C81" s="114"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="320"/>
-      <c r="B82" s="320"/>
+      <c r="A82" s="315"/>
+      <c r="B82" s="315"/>
       <c r="C82" s="114"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="316"/>
-      <c r="B83" s="316"/>
+      <c r="A83" s="314"/>
+      <c r="B83" s="314"/>
       <c r="C83" s="110"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="316"/>
-      <c r="B84" s="316"/>
+      <c r="A84" s="314"/>
+      <c r="B84" s="314"/>
       <c r="C84" s="110"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="316"/>
-      <c r="B85" s="316"/>
+      <c r="A85" s="314"/>
+      <c r="B85" s="314"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="316"/>
-      <c r="B86" s="316"/>
+      <c r="A86" s="314"/>
+      <c r="B86" s="314"/>
       <c r="C86" s="111"/>
       <c r="D86" s="111"/>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="316"/>
-      <c r="B87" s="316"/>
+      <c r="A87" s="314"/>
+      <c r="B87" s="314"/>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="319"/>
-      <c r="B88" s="319"/>
+      <c r="A88" s="313"/>
+      <c r="B88" s="313"/>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="316"/>
-      <c r="B89" s="316"/>
+      <c r="A89" s="314"/>
+      <c r="B89" s="314"/>
       <c r="C89" s="114"/>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="316"/>
-      <c r="B90" s="316"/>
+      <c r="A90" s="314"/>
+      <c r="B90" s="314"/>
       <c r="C90" s="114"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="320"/>
-      <c r="B91" s="320"/>
+      <c r="A91" s="315"/>
+      <c r="B91" s="315"/>
       <c r="C91" s="115"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="316"/>
-      <c r="B92" s="316"/>
+      <c r="A92" s="314"/>
+      <c r="B92" s="314"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A73:B73"/>
     <mergeCell ref="A87:B87"/>
     <mergeCell ref="A75:B75"/>
     <mergeCell ref="A76:B76"/>
@@ -17196,50 +17235,11 @@
     <mergeCell ref="A84:B84"/>
     <mergeCell ref="A85:B85"/>
     <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -17250,8 +17250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CAAAA1-AE59-4B49-86BC-C8B3BF8E138F}">
   <dimension ref="A1:BM454"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17301,24 +17301,24 @@
       <c r="B2" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="328"/>
-      <c r="D2" s="326"/>
-      <c r="E2" s="326"/>
-      <c r="F2" s="327"/>
+      <c r="C2" s="327"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="329"/>
       <c r="G2" s="15"/>
       <c r="H2" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="324"/>
-      <c r="J2" s="324"/>
-      <c r="K2" s="325"/>
+      <c r="I2" s="330"/>
+      <c r="J2" s="330"/>
+      <c r="K2" s="331"/>
       <c r="L2" s="15"/>
       <c r="M2" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="N2" s="324"/>
-      <c r="O2" s="324"/>
-      <c r="P2" s="325"/>
+      <c r="N2" s="330"/>
+      <c r="O2" s="330"/>
+      <c r="P2" s="331"/>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -18269,9 +18269,9 @@
       <c r="M12" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N12" s="324"/>
-      <c r="O12" s="324"/>
-      <c r="P12" s="325"/>
+      <c r="N12" s="330"/>
+      <c r="O12" s="330"/>
+      <c r="P12" s="331"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
       <c r="S12" s="15"/>
@@ -19965,24 +19965,24 @@
       <c r="B32" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="326"/>
-      <c r="D32" s="326"/>
-      <c r="E32" s="326"/>
-      <c r="F32" s="327"/>
+      <c r="C32" s="328"/>
+      <c r="D32" s="328"/>
+      <c r="E32" s="328"/>
+      <c r="F32" s="329"/>
       <c r="G32" s="15"/>
       <c r="H32" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="324"/>
-      <c r="J32" s="324"/>
-      <c r="K32" s="325"/>
+      <c r="I32" s="330"/>
+      <c r="J32" s="330"/>
+      <c r="K32" s="331"/>
       <c r="L32" s="15"/>
       <c r="M32" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="N32" s="324"/>
-      <c r="O32" s="324"/>
-      <c r="P32" s="325"/>
+      <c r="N32" s="330"/>
+      <c r="O32" s="330"/>
+      <c r="P32" s="331"/>
       <c r="Q32" s="15"/>
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
@@ -20882,9 +20882,9 @@
       <c r="M42" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N42" s="324"/>
-      <c r="O42" s="324"/>
-      <c r="P42" s="325"/>
+      <c r="N42" s="330"/>
+      <c r="O42" s="330"/>
+      <c r="P42" s="331"/>
       <c r="Q42" s="15"/>
       <c r="R42" s="15"/>
       <c r="S42" s="15"/>
@@ -22519,24 +22519,24 @@
       <c r="B62" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C62" s="326"/>
-      <c r="D62" s="326"/>
-      <c r="E62" s="326"/>
-      <c r="F62" s="327"/>
+      <c r="C62" s="328"/>
+      <c r="D62" s="328"/>
+      <c r="E62" s="328"/>
+      <c r="F62" s="329"/>
       <c r="G62" s="15"/>
       <c r="H62" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="I62" s="324"/>
-      <c r="J62" s="324"/>
-      <c r="K62" s="325"/>
+      <c r="I62" s="330"/>
+      <c r="J62" s="330"/>
+      <c r="K62" s="331"/>
       <c r="L62" s="15"/>
       <c r="M62" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="N62" s="324"/>
-      <c r="O62" s="324"/>
-      <c r="P62" s="325"/>
+      <c r="N62" s="330"/>
+      <c r="O62" s="330"/>
+      <c r="P62" s="331"/>
       <c r="Q62" s="15"/>
       <c r="R62" s="15"/>
       <c r="S62" s="15"/>
@@ -23487,9 +23487,9 @@
       <c r="M72" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="N72" s="324"/>
-      <c r="O72" s="324"/>
-      <c r="P72" s="325"/>
+      <c r="N72" s="330"/>
+      <c r="O72" s="330"/>
+      <c r="P72" s="331"/>
       <c r="Q72" s="15"/>
       <c r="R72" s="15"/>
       <c r="S72" s="15"/>
@@ -25128,10 +25128,10 @@
     <row r="91" spans="1:65" ht="18.75" thickBot="1">
       <c r="A91" s="15"/>
       <c r="B91" s="23"/>
-      <c r="C91" s="321"/>
-      <c r="D91" s="322"/>
-      <c r="E91" s="322"/>
-      <c r="F91" s="323"/>
+      <c r="C91" s="332"/>
+      <c r="D91" s="333"/>
+      <c r="E91" s="333"/>
+      <c r="F91" s="334"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15"/>
       <c r="I91" s="15"/>
@@ -25194,7 +25194,7 @@
     </row>
     <row r="92" spans="1:65" ht="18">
       <c r="A92" s="15"/>
-      <c r="B92" s="334" t="s">
+      <c r="B92" s="301" t="s">
         <v>240</v>
       </c>
       <c r="C92" s="179" t="s">
@@ -25286,7 +25286,7 @@
         <f t="shared" si="43"/>
         <v>-3294</v>
       </c>
-      <c r="F93" s="331">
+      <c r="F93" s="298">
         <f t="shared" si="43"/>
         <v>-7395</v>
       </c>
@@ -25367,7 +25367,7 @@
         <f t="shared" si="44"/>
         <v>0.91315581334036378</v>
       </c>
-      <c r="F94" s="332">
+      <c r="F94" s="299">
         <f t="shared" si="44"/>
         <v>0.83518320406525814</v>
       </c>
@@ -25448,7 +25448,7 @@
         <f>(CashY3+E7)/E17</f>
         <v>0.73416820458739784</v>
       </c>
-      <c r="F95" s="332">
+      <c r="F95" s="299">
         <f>(CashY4+F7)/F17</f>
         <v>0.62456539181599358</v>
       </c>
@@ -25526,7 +25526,7 @@
         <f t="shared" ref="E96:F96" si="45">J$6/E7</f>
         <v>5.2132499402438048</v>
       </c>
-      <c r="F96" s="332">
+      <c r="F96" s="299">
         <f t="shared" si="45"/>
         <v>5.1857328247276735</v>
       </c>
@@ -25604,7 +25604,7 @@
         <f t="shared" ref="E97:F97" si="46">365/E96</f>
         <v>70.013907674438158</v>
       </c>
-      <c r="F97" s="332">
+      <c r="F97" s="299">
         <f t="shared" si="46"/>
         <v>70.385423302089961</v>
       </c>
@@ -25682,7 +25682,7 @@
         <f t="shared" ref="E98:F98" si="47">J$6/E6</f>
         <v>97.95134730538922</v>
       </c>
-      <c r="F98" s="332">
+      <c r="F98" s="299">
         <f t="shared" si="47"/>
         <v>92.734177215189874</v>
       </c>
@@ -25760,7 +25760,7 @@
         <f t="shared" ref="E99:F99" si="48">E98*365</f>
         <v>35752.241766467065</v>
       </c>
-      <c r="F99" s="333">
+      <c r="F99" s="300">
         <f t="shared" si="48"/>
         <v>33847.974683544307</v>
       </c>
@@ -25832,7 +25832,7 @@
       <c r="C100" s="293"/>
       <c r="D100" s="293"/>
       <c r="E100" s="293"/>
-      <c r="F100" s="332"/>
+      <c r="F100" s="299"/>
       <c r="G100" s="15"/>
       <c r="H100" s="15"/>
       <c r="I100" s="15"/>
@@ -25901,7 +25901,7 @@
       <c r="C101" s="293"/>
       <c r="D101" s="293"/>
       <c r="E101" s="293"/>
-      <c r="F101" s="332"/>
+      <c r="F101" s="299"/>
       <c r="G101" s="15"/>
       <c r="H101" s="15"/>
       <c r="I101" s="15"/>
@@ -25970,7 +25970,7 @@
       <c r="C102" s="293"/>
       <c r="D102" s="293"/>
       <c r="E102" s="293"/>
-      <c r="F102" s="332"/>
+      <c r="F102" s="299"/>
       <c r="G102" s="15"/>
       <c r="H102" s="15"/>
       <c r="I102" s="15"/>
@@ -26045,7 +26045,7 @@
         <f t="shared" ref="E103:F103" si="49">J$6/E10</f>
         <v>1.4656609098850883</v>
       </c>
-      <c r="F103" s="332">
+      <c r="F103" s="299">
         <f t="shared" si="49"/>
         <v>1.4346733394984497</v>
       </c>
@@ -26126,7 +26126,7 @@
         <f>TotalLiabilitiesY3/TotalAssetsY3</f>
         <v>0.79341386328536523</v>
       </c>
-      <c r="F104" s="332">
+      <c r="F104" s="299">
         <f>TotalLiabilitiesY4/TotalAssetsY4</f>
         <v>0.78461026919003041</v>
       </c>
@@ -26204,7 +26204,7 @@
         <f>J17/AVERAGE(D28:E28)</f>
         <v>0.32272603800919547</v>
       </c>
-      <c r="F105" s="332">
+      <c r="F105" s="299">
         <f t="shared" ref="F105" si="50">K17/AVERAGE(E28:F28)</f>
         <v>0.33668807690671659</v>
       </c>
@@ -26281,7 +26281,7 @@
         <f>J17/AVERAGE(TotalAssetsY2, TotalAssetsY3)</f>
         <v>6.1455403738131548E-2</v>
       </c>
-      <c r="F106" s="332">
+      <c r="F106" s="299">
         <f>K17/AVERAGE(TotalAssetsY3, TotalAssetsY4)</f>
         <v>7.1108747367740172E-2</v>
       </c>
@@ -26358,7 +26358,7 @@
         <f t="shared" ref="E107:F107" si="51">J8/J$6</f>
         <v>0.57583121279506044</v>
       </c>
-      <c r="F107" s="332">
+      <c r="F107" s="299">
         <f t="shared" si="51"/>
         <v>0.58499408499408501</v>
       </c>
@@ -26436,7 +26436,7 @@
         <f t="shared" ref="E108:F108" si="52">J10/J6</f>
         <v>0.27260570214651964</v>
       </c>
-      <c r="F108" s="332">
+      <c r="F108" s="299">
         <f t="shared" si="52"/>
         <v>0.22812206145539479</v>
       </c>
@@ -26514,7 +26514,7 @@
         <f t="shared" ref="E109:F109" si="53">J11/J6</f>
         <v>0.17023910501822517</v>
       </c>
-      <c r="F109" s="332">
+      <c r="F109" s="299">
         <f t="shared" si="53"/>
         <v>0.23036673036673036</v>
       </c>
@@ -26592,7 +26592,7 @@
         <f t="shared" ref="E110:F110" si="54">J17/J6</f>
         <v>0.12256329138106264</v>
       </c>
-      <c r="F110" s="332">
+      <c r="F110" s="299">
         <f t="shared" si="54"/>
         <v>0.15005915005915005</v>
       </c>
@@ -26670,7 +26670,7 @@
         <f t="shared" ref="E111:F111" si="55">J18</f>
         <v>3.76</v>
       </c>
-      <c r="F111" s="331">
+      <c r="F111" s="298">
         <f t="shared" si="55"/>
         <v>4.66</v>
       </c>
@@ -26748,7 +26748,7 @@
         <f t="shared" ref="E112:F112" si="56">O19</f>
         <v>2.3649564375605032</v>
       </c>
-      <c r="F112" s="331">
+      <c r="F112" s="298">
         <f t="shared" si="56"/>
         <v>2.4193236714975845</v>
       </c>
@@ -26826,7 +26826,7 @@
         <f>J6/(AVERAGE(TotalAssetsY2+TotalAssetsY3))</f>
         <v>0.25070885028315693</v>
       </c>
-      <c r="F113" s="332">
+      <c r="F113" s="299">
         <f>K6/(AVERAGE(TotalAssetsY3+TotalAssetsY4))</f>
         <v>0.23693572614435923</v>
       </c>
@@ -26904,7 +26904,7 @@
         <f>E113*E110</f>
         <v>3.0727701869065774E-2</v>
       </c>
-      <c r="F114" s="332">
+      <c r="F114" s="299">
         <f>F113*F110</f>
         <v>3.5554373683870086E-2</v>
       </c>
@@ -26982,7 +26982,7 @@
         <f>(AVERAGE(TotalAssetsY2+TotalAssetsY3))/(AVERAGE(D28:E28))</f>
         <v>10.502771713431995</v>
       </c>
-      <c r="F115" s="332">
+      <c r="F115" s="299">
         <f>(AVERAGE(TotalAssetsY3+TotalAssetsY4))/(AVERAGE(E28:F28))</f>
         <v>9.4696669360670374</v>
       </c>
@@ -27060,7 +27060,7 @@
         <f t="shared" ref="E116:F116" si="57">E115*E114</f>
         <v>0.32272603800919547</v>
       </c>
-      <c r="F116" s="332">
+      <c r="F116" s="299">
         <f t="shared" si="57"/>
         <v>0.33668807690671654</v>
       </c>
@@ -27126,13 +27126,13 @@
     </row>
     <row r="117" spans="1:65" ht="15.75">
       <c r="A117" s="15"/>
-      <c r="B117" s="335" t="s">
+      <c r="B117" s="302" t="s">
         <v>262</v>
       </c>
-      <c r="C117" s="336"/>
-      <c r="D117" s="336"/>
-      <c r="E117" s="336"/>
-      <c r="F117" s="336"/>
+      <c r="C117" s="303"/>
+      <c r="D117" s="303"/>
+      <c r="E117" s="303"/>
+      <c r="F117" s="303"/>
       <c r="G117" s="15"/>
       <c r="H117" s="15"/>
       <c r="I117" s="15"/>
@@ -49434,6 +49434,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C91:F91"/>
+    <mergeCell ref="N72:P72"/>
+    <mergeCell ref="N62:P62"/>
+    <mergeCell ref="I62:K62"/>
+    <mergeCell ref="C62:F62"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="N2:P2"/>
@@ -49442,11 +49447,6 @@
     <mergeCell ref="N32:P32"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C91:F91"/>
-    <mergeCell ref="N72:P72"/>
-    <mergeCell ref="N62:P62"/>
-    <mergeCell ref="I62:K62"/>
-    <mergeCell ref="C62:F62"/>
   </mergeCells>
   <conditionalFormatting sqref="C40:F40">
     <cfRule type="colorScale" priority="28">
@@ -50201,18 +50201,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="329" t="s">
+      <c r="A1" s="335" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="330" t="s">
+      <c r="B1" s="336" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="330"/>
-      <c r="D1" s="330"/>
+      <c r="C1" s="336"/>
+      <c r="D1" s="336"/>
       <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="316"/>
+      <c r="A2" s="314"/>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
@@ -51342,18 +51342,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="A1" s="329" t="s">
+      <c r="A1" s="335" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="330" t="s">
+      <c r="B1" s="336" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="330"/>
-      <c r="D1" s="330"/>
+      <c r="C1" s="336"/>
+      <c r="D1" s="336"/>
       <c r="E1" s="63"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="316"/>
+      <c r="A2" s="314"/>
       <c r="B2" s="10" t="s">
         <v>4</v>
       </c>

</xml_diff>